<commit_message>
Updates to EAF Makros and UDAs
</commit_message>
<xml_diff>
--- a/EXCEL/UDAGEN.xlsx
+++ b/EXCEL/UDAGEN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MAC\MACROS_WORK\EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4705E177-0C14-4B0F-8476-BF7992047F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77E6870-582C-4CC8-B7AE-A1AEE5137872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44550" yWindow="0" windowWidth="28800" windowHeight="18555" activeTab="1" xr2:uid="{97B28DAE-2167-4984-9CE6-3AC0C30C0AA5}"/>
+    <workbookView xWindow="44295" yWindow="1275" windowWidth="28800" windowHeight="17550" xr2:uid="{97B28DAE-2167-4984-9CE6-3AC0C30C0AA5}"/>
   </bookViews>
   <sheets>
     <sheet name="UDA" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="342">
   <si>
     <t>Content</t>
   </si>
@@ -1053,6 +1053,18 @@
   </si>
   <si>
     <t>Leistung [kW]</t>
+  </si>
+  <si>
+    <t>Weight Valve Drive</t>
+  </si>
+  <si>
+    <t>Weight Valve No Drive</t>
+  </si>
+  <si>
+    <t>Gewicht ohne Antrieb [mm]</t>
+  </si>
+  <si>
+    <t>Gewicht von Antrieb [mm]</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1242,8 +1254,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2221,7 +2231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83F1353-7DE5-45CC-8469-BC8D38DE6EDF}">
   <dimension ref="A1:R85"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
       <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
@@ -7662,32 +7672,38 @@
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A79" s="6"/>
+      <c r="A79" s="6" t="s">
+        <v>339</v>
+      </c>
       <c r="B79" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Remain[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
-        <v/>
+        <v>WeightValveNoDrive</v>
       </c>
       <c r="C79" s="6" t="str">
         <f>Remain[[#Headers],[new uda /]]</f>
         <v>new uda /</v>
       </c>
-      <c r="D79" s="6"/>
-      <c r="E79" s="6"/>
+      <c r="D79" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>340</v>
+      </c>
       <c r="F79" s="6" t="str">
         <f>Remain[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
       <c r="G79" s="6" t="str">
         <f>"Tg"&amp;Remain[[#This Row],[UDET desc]]&amp;Remain[[#This Row],[Desc E3D]]</f>
-        <v>Tg</v>
+        <v>TgValveWeightValveNoDrive</v>
       </c>
       <c r="H79" s="6" t="str">
         <f t="shared" si="31"/>
-        <v>TgUDA</v>
+        <v>TgValveWeightValveNoDriveUDA</v>
       </c>
       <c r="I79" s="6" t="str">
         <f t="shared" si="32"/>
-        <v>Ablength 2</v>
+        <v>Ablength 25</v>
       </c>
       <c r="J79" s="6" t="str">
         <f>Remain[[#Headers],[Ulength 250]]</f>
@@ -7702,56 +7718,62 @@
       </c>
       <c r="M79" s="6" t="str">
         <f t="shared" si="33"/>
-        <v>udname 'Tg'</v>
+        <v>udname 'TgValveWeightValveNoDrive'</v>
       </c>
       <c r="N79" s="6" t="str">
         <f>"Rptxt '"&amp;Remain[[#This Row],[UDA desc]]&amp;"'"</f>
-        <v>Rptxt ''</v>
+        <v>Rptxt 'Gewicht ohne Antrieb [mm]'</v>
       </c>
       <c r="O79" s="6" t="str">
         <f>"desc '"&amp;Remain[[#This Row],[UDA desc]]&amp;"'"</f>
-        <v>desc ''</v>
+        <v>desc 'Gewicht ohne Antrieb [mm]'</v>
       </c>
       <c r="P79" s="6" t="str">
         <f t="shared" si="34"/>
-        <v>new uda /TgUDA utype text Ablength 2 Ulength 250 Elelist :TgObValve udname 'Tg' Rptxt '' desc ''</v>
+        <v>new uda /TgValveWeightValveNoDriveUDA utype text Ablength 25 Ulength 250 Elelist :TgObValve udname 'TgValveWeightValveNoDrive' Rptxt 'Gewicht ohne Antrieb [mm]' desc 'Gewicht ohne Antrieb [mm]'</v>
       </c>
       <c r="Q79" s="6" t="str">
         <f t="shared" si="35"/>
-        <v>new attcol DbAttribute :Tg</v>
+        <v>new attcol DbAttribute :TgValveWeightValveNoDrive</v>
       </c>
       <c r="R79" s="6" t="str">
         <f t="shared" si="36"/>
-        <v>/TgUDA Rptxt '' desc ''</v>
+        <v>/TgValveWeightValveNoDriveUDA Rptxt 'Gewicht ohne Antrieb [mm]' desc 'Gewicht ohne Antrieb [mm]'</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A80" s="6"/>
+      <c r="A80" s="6" t="s">
+        <v>338</v>
+      </c>
       <c r="B80" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Remain[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
-        <v/>
+        <v>WeightValveDrive</v>
       </c>
       <c r="C80" s="6" t="str">
         <f>Remain[[#Headers],[new uda /]]</f>
         <v>new uda /</v>
       </c>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
+      <c r="D80" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>341</v>
+      </c>
       <c r="F80" s="6" t="str">
         <f>Remain[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
       <c r="G80" s="6" t="str">
         <f>"Tg"&amp;Remain[[#This Row],[UDET desc]]&amp;Remain[[#This Row],[Desc E3D]]</f>
-        <v>Tg</v>
+        <v>TgValveWeightValveDrive</v>
       </c>
       <c r="H80" s="6" t="str">
         <f t="shared" si="31"/>
-        <v>TgUDA</v>
+        <v>TgValveWeightValveDriveUDA</v>
       </c>
       <c r="I80" s="6" t="str">
         <f t="shared" si="32"/>
-        <v>Ablength 2</v>
+        <v>Ablength 23</v>
       </c>
       <c r="J80" s="6" t="str">
         <f>Remain[[#Headers],[Ulength 250]]</f>
@@ -7766,27 +7788,27 @@
       </c>
       <c r="M80" s="6" t="str">
         <f t="shared" si="33"/>
-        <v>udname 'Tg'</v>
+        <v>udname 'TgValveWeightValveDrive'</v>
       </c>
       <c r="N80" s="6" t="str">
         <f>"Rptxt '"&amp;Remain[[#This Row],[UDA desc]]&amp;"'"</f>
-        <v>Rptxt ''</v>
+        <v>Rptxt 'Gewicht von Antrieb [mm]'</v>
       </c>
       <c r="O80" s="6" t="str">
         <f>"desc '"&amp;Remain[[#This Row],[UDA desc]]&amp;"'"</f>
-        <v>desc ''</v>
+        <v>desc 'Gewicht von Antrieb [mm]'</v>
       </c>
       <c r="P80" s="6" t="str">
         <f t="shared" si="34"/>
-        <v>new uda /TgUDA utype text Ablength 2 Ulength 250 Elelist :TgObValve udname 'Tg' Rptxt '' desc ''</v>
+        <v>new uda /TgValveWeightValveDriveUDA utype text Ablength 23 Ulength 250 Elelist :TgObValve udname 'TgValveWeightValveDrive' Rptxt 'Gewicht von Antrieb [mm]' desc 'Gewicht von Antrieb [mm]'</v>
       </c>
       <c r="Q80" s="6" t="str">
         <f t="shared" si="35"/>
-        <v>new attcol DbAttribute :Tg</v>
+        <v>new attcol DbAttribute :TgValveWeightValveDrive</v>
       </c>
       <c r="R80" s="6" t="str">
         <f t="shared" si="36"/>
-        <v>/TgUDA Rptxt '' desc ''</v>
+        <v>/TgValveWeightValveDriveUDA Rptxt 'Gewicht von Antrieb [mm]' desc 'Gewicht von Antrieb [mm]'</v>
       </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
@@ -8122,7 +8144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97400A6C-8E9E-4F62-8A84-B939A5F5F2BE}">
   <dimension ref="A1:R78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H52" sqref="H52:H78"/>
     </sheetView>
   </sheetViews>
@@ -12182,7 +12204,7 @@
       <c r="A59" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="B59" s="23" t="str">
+      <c r="B59" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>MinimumPermittedMassFlowContinuous</v>
       </c>
@@ -12200,7 +12222,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G59" s="24" t="str">
+      <c r="G59" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpMinimumPermittedMassFlowContinuous</v>
       </c>
@@ -12227,11 +12249,11 @@
         <f t="shared" ref="M59:M78" si="11">"udname '"&amp;G59&amp;"'"</f>
         <v>udname 'TgPumpMinimumPermittedMassFlowContinuous'</v>
       </c>
-      <c r="N59" s="24" t="str">
+      <c r="N59" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'mind. zul. Förderstrom für stabilen Dauerbetrieb [m3/h]'</v>
       </c>
-      <c r="O59" s="24" t="str">
+      <c r="O59" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'mind. zul. Förderstrom für stabilen Dauerbetrieb [m3/h]'</v>
       </c>
@@ -12243,7 +12265,7 @@
         <f t="shared" ref="Q59:Q78" si="13">"new attcol DbAttribute :"&amp;$G59</f>
         <v>new attcol DbAttribute :TgPumpMinimumPermittedMassFlowContinuous</v>
       </c>
-      <c r="R59" s="24" t="str">
+      <c r="R59" s="6" t="str">
         <f t="shared" ref="R59:R78" si="14">CONCATENATE("/",$H59," ",$N59," ",$O59)</f>
         <v>/TgPumpMinimumPermittedMassFlowContinuousUDA Rptxt 'mind. zul. Förderstrom für stabilen Dauerbetrieb [m3/h]' desc 'mind. zul. Förderstrom für stabilen Dauerbetrieb [m3/h]'</v>
       </c>
@@ -12252,7 +12274,7 @@
       <c r="A60" s="22" t="s">
         <v>291</v>
       </c>
-      <c r="B60" s="23" t="str">
+      <c r="B60" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>PumpStandard</v>
       </c>
@@ -12270,7 +12292,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G60" s="24" t="str">
+      <c r="G60" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpPumpStandard</v>
       </c>
@@ -12297,11 +12319,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpPumpStandard'</v>
       </c>
-      <c r="N60" s="24" t="str">
+      <c r="N60" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'Pumpennorm'</v>
       </c>
-      <c r="O60" s="24" t="str">
+      <c r="O60" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'Pumpennorm'</v>
       </c>
@@ -12313,7 +12335,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpPumpStandard</v>
       </c>
-      <c r="R60" s="24" t="str">
+      <c r="R60" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpPumpStandardUDA Rptxt 'Pumpennorm' desc 'Pumpennorm'</v>
       </c>
@@ -12322,7 +12344,7 @@
       <c r="A61" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="B61" s="23" t="str">
+      <c r="B61" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>Execution</v>
       </c>
@@ -12340,7 +12362,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G61" s="24" t="str">
+      <c r="G61" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpExecution</v>
       </c>
@@ -12367,11 +12389,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpExecution'</v>
       </c>
-      <c r="N61" s="24" t="str">
+      <c r="N61" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'Ausführung'</v>
       </c>
-      <c r="O61" s="24" t="str">
+      <c r="O61" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'Ausführung'</v>
       </c>
@@ -12383,7 +12405,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpExecution</v>
       </c>
-      <c r="R61" s="24" t="str">
+      <c r="R61" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpExecutionUDA Rptxt 'Ausführung' desc 'Ausführung'</v>
       </c>
@@ -12392,7 +12414,7 @@
       <c r="A62" s="22" t="s">
         <v>293</v>
       </c>
-      <c r="B62" s="23" t="str">
+      <c r="B62" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>ShaftExecution</v>
       </c>
@@ -12410,7 +12432,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G62" s="24" t="str">
+      <c r="G62" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpShaftExecution</v>
       </c>
@@ -12437,11 +12459,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpShaftExecution'</v>
       </c>
-      <c r="N62" s="24" t="str">
+      <c r="N62" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'Wellenausführung'</v>
       </c>
-      <c r="O62" s="24" t="str">
+      <c r="O62" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'Wellenausführung'</v>
       </c>
@@ -12453,7 +12475,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpShaftExecution</v>
       </c>
-      <c r="R62" s="24" t="str">
+      <c r="R62" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpShaftExecutionUDA Rptxt 'Wellenausführung' desc 'Wellenausführung'</v>
       </c>
@@ -12462,7 +12484,7 @@
       <c r="A63" s="21" t="s">
         <v>294</v>
       </c>
-      <c r="B63" s="23" t="str">
+      <c r="B63" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>NominalPressure</v>
       </c>
@@ -12480,7 +12502,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G63" s="24" t="str">
+      <c r="G63" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpNominalPressure</v>
       </c>
@@ -12507,11 +12529,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpNominalPressure'</v>
       </c>
-      <c r="N63" s="24" t="str">
+      <c r="N63" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'Nenndruck'</v>
       </c>
-      <c r="O63" s="24" t="str">
+      <c r="O63" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'Nenndruck'</v>
       </c>
@@ -12523,7 +12545,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpNominalPressure</v>
       </c>
-      <c r="R63" s="24" t="str">
+      <c r="R63" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpNominalPressureUDA Rptxt 'Nenndruck' desc 'Nenndruck'</v>
       </c>
@@ -12532,7 +12554,7 @@
       <c r="A64" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="B64" s="23" t="str">
+      <c r="B64" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>InletNominalDiameter</v>
       </c>
@@ -12550,7 +12572,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G64" s="24" t="str">
+      <c r="G64" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpInletNominalDiameter</v>
       </c>
@@ -12577,11 +12599,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpInletNominalDiameter'</v>
       </c>
-      <c r="N64" s="24" t="str">
+      <c r="N64" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'DN Saugstutzen'</v>
       </c>
-      <c r="O64" s="24" t="str">
+      <c r="O64" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'DN Saugstutzen'</v>
       </c>
@@ -12593,7 +12615,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpInletNominalDiameter</v>
       </c>
-      <c r="R64" s="24" t="str">
+      <c r="R64" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpInletNominalDiameterUDA Rptxt 'DN Saugstutzen' desc 'DN Saugstutzen'</v>
       </c>
@@ -12602,7 +12624,7 @@
       <c r="A65" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="B65" s="23" t="str">
+      <c r="B65" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>InletNominalPressure</v>
       </c>
@@ -12620,7 +12642,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G65" s="24" t="str">
+      <c r="G65" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpInletNominalPressure</v>
       </c>
@@ -12647,11 +12669,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpInletNominalPressure'</v>
       </c>
-      <c r="N65" s="24" t="str">
+      <c r="N65" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'PN Saugstutzen'</v>
       </c>
-      <c r="O65" s="24" t="str">
+      <c r="O65" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'PN Saugstutzen'</v>
       </c>
@@ -12663,7 +12685,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpInletNominalPressure</v>
       </c>
-      <c r="R65" s="24" t="str">
+      <c r="R65" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpInletNominalPressureUDA Rptxt 'PN Saugstutzen' desc 'PN Saugstutzen'</v>
       </c>
@@ -12672,7 +12694,7 @@
       <c r="A66" s="22" t="s">
         <v>297</v>
       </c>
-      <c r="B66" s="23" t="str">
+      <c r="B66" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>InletStandard</v>
       </c>
@@ -12690,7 +12712,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G66" s="24" t="str">
+      <c r="G66" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpInletStandard</v>
       </c>
@@ -12717,11 +12739,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpInletStandard'</v>
       </c>
-      <c r="N66" s="24" t="str">
+      <c r="N66" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'Norm Saugflansch'</v>
       </c>
-      <c r="O66" s="24" t="str">
+      <c r="O66" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'Norm Saugflansch'</v>
       </c>
@@ -12733,7 +12755,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpInletStandard</v>
       </c>
-      <c r="R66" s="24" t="str">
+      <c r="R66" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpInletStandardUDA Rptxt 'Norm Saugflansch' desc 'Norm Saugflansch'</v>
       </c>
@@ -12742,7 +12764,7 @@
       <c r="A67" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="B67" s="23" t="str">
+      <c r="B67" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>DischargeNominalDiameter</v>
       </c>
@@ -12760,7 +12782,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G67" s="24" t="str">
+      <c r="G67" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpDischargeNominalDiameter</v>
       </c>
@@ -12787,11 +12809,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpDischargeNominalDiameter'</v>
       </c>
-      <c r="N67" s="24" t="str">
+      <c r="N67" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'DN Druckstutzen'</v>
       </c>
-      <c r="O67" s="24" t="str">
+      <c r="O67" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'DN Druckstutzen'</v>
       </c>
@@ -12803,7 +12825,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpDischargeNominalDiameter</v>
       </c>
-      <c r="R67" s="24" t="str">
+      <c r="R67" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpDischargeNominalDiameterUDA Rptxt 'DN Druckstutzen' desc 'DN Druckstutzen'</v>
       </c>
@@ -12812,7 +12834,7 @@
       <c r="A68" s="22" t="s">
         <v>299</v>
       </c>
-      <c r="B68" s="23" t="str">
+      <c r="B68" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>DischargeNominalPressure</v>
       </c>
@@ -12830,7 +12852,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G68" s="24" t="str">
+      <c r="G68" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpDischargeNominalPressure</v>
       </c>
@@ -12857,11 +12879,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpDischargeNominalPressure'</v>
       </c>
-      <c r="N68" s="24" t="str">
+      <c r="N68" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'PN Druckstutzen'</v>
       </c>
-      <c r="O68" s="24" t="str">
+      <c r="O68" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'PN Druckstutzen'</v>
       </c>
@@ -12873,7 +12895,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpDischargeNominalPressure</v>
       </c>
-      <c r="R68" s="24" t="str">
+      <c r="R68" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpDischargeNominalPressureUDA Rptxt 'PN Druckstutzen' desc 'PN Druckstutzen'</v>
       </c>
@@ -12882,7 +12904,7 @@
       <c r="A69" s="21" t="s">
         <v>300</v>
       </c>
-      <c r="B69" s="23" t="str">
+      <c r="B69" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>DischargeStandard</v>
       </c>
@@ -12900,7 +12922,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G69" s="24" t="str">
+      <c r="G69" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpDischargeStandard</v>
       </c>
@@ -12927,11 +12949,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpDischargeStandard'</v>
       </c>
-      <c r="N69" s="24" t="str">
+      <c r="N69" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'Norm Druckflansch'</v>
       </c>
-      <c r="O69" s="24" t="str">
+      <c r="O69" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'Norm Druckflansch'</v>
       </c>
@@ -12943,7 +12965,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpDischargeStandard</v>
       </c>
-      <c r="R69" s="24" t="str">
+      <c r="R69" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpDischargeStandardUDA Rptxt 'Norm Druckflansch' desc 'Norm Druckflansch'</v>
       </c>
@@ -12952,7 +12974,7 @@
       <c r="A70" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="B70" s="23" t="str">
+      <c r="B70" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>SealType</v>
       </c>
@@ -12970,7 +12992,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G70" s="24" t="str">
+      <c r="G70" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpSealType</v>
       </c>
@@ -12997,11 +13019,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpSealType'</v>
       </c>
-      <c r="N70" s="24" t="str">
+      <c r="N70" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'Art Dichtung'</v>
       </c>
-      <c r="O70" s="24" t="str">
+      <c r="O70" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'Art Dichtung'</v>
       </c>
@@ -13013,7 +13035,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpSealType</v>
       </c>
-      <c r="R70" s="24" t="str">
+      <c r="R70" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpSealTypeUDA Rptxt 'Art Dichtung' desc 'Art Dichtung'</v>
       </c>
@@ -13022,7 +13044,7 @@
       <c r="A71" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="B71" s="23" t="str">
+      <c r="B71" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>SealManufacturer</v>
       </c>
@@ -13040,7 +13062,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G71" s="24" t="str">
+      <c r="G71" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpSealManufacturer</v>
       </c>
@@ -13067,11 +13089,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpSealManufacturer'</v>
       </c>
-      <c r="N71" s="24" t="str">
+      <c r="N71" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'Hersteller Dichtung'</v>
       </c>
-      <c r="O71" s="24" t="str">
+      <c r="O71" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'Hersteller Dichtung'</v>
       </c>
@@ -13083,7 +13105,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpSealManufacturer</v>
       </c>
-      <c r="R71" s="24" t="str">
+      <c r="R71" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpSealManufacturerUDA Rptxt 'Hersteller Dichtung' desc 'Hersteller Dichtung'</v>
       </c>
@@ -13092,7 +13114,7 @@
       <c r="A72" s="22" t="s">
         <v>303</v>
       </c>
-      <c r="B72" s="23" t="str">
+      <c r="B72" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>SealModel</v>
       </c>
@@ -13110,7 +13132,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G72" s="24" t="str">
+      <c r="G72" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpSealModel</v>
       </c>
@@ -13137,11 +13159,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpSealModel'</v>
       </c>
-      <c r="N72" s="24" t="str">
+      <c r="N72" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'Type Dichtung'</v>
       </c>
-      <c r="O72" s="24" t="str">
+      <c r="O72" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'Type Dichtung'</v>
       </c>
@@ -13153,7 +13175,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpSealModel</v>
       </c>
-      <c r="R72" s="24" t="str">
+      <c r="R72" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpSealModelUDA Rptxt 'Type Dichtung' desc 'Type Dichtung'</v>
       </c>
@@ -13162,7 +13184,7 @@
       <c r="A73" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="B73" s="23" t="str">
+      <c r="B73" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>ImpellerDiameter</v>
       </c>
@@ -13180,7 +13202,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G73" s="24" t="str">
+      <c r="G73" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpImpellerDiameter</v>
       </c>
@@ -13207,11 +13229,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpImpellerDiameter'</v>
       </c>
-      <c r="N73" s="24" t="str">
+      <c r="N73" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'Laufraddurchmesser [mm]'</v>
       </c>
-      <c r="O73" s="24" t="str">
+      <c r="O73" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'Laufraddurchmesser [mm]'</v>
       </c>
@@ -13223,7 +13245,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpImpellerDiameter</v>
       </c>
-      <c r="R73" s="24" t="str">
+      <c r="R73" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpImpellerDiameterUDA Rptxt 'Laufraddurchmesser [mm]' desc 'Laufraddurchmesser [mm]'</v>
       </c>
@@ -13232,7 +13254,7 @@
       <c r="A74" s="22" t="s">
         <v>305</v>
       </c>
-      <c r="B74" s="23" t="str">
+      <c r="B74" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>BearingSeal</v>
       </c>
@@ -13250,7 +13272,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G74" s="24" t="str">
+      <c r="G74" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpBearingSeal</v>
       </c>
@@ -13277,11 +13299,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpBearingSeal'</v>
       </c>
-      <c r="N74" s="24" t="str">
+      <c r="N74" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'Lagerdichtung'</v>
       </c>
-      <c r="O74" s="24" t="str">
+      <c r="O74" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'Lagerdichtung'</v>
       </c>
@@ -13293,7 +13315,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpBearingSeal</v>
       </c>
-      <c r="R74" s="24" t="str">
+      <c r="R74" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpBearingSealUDA Rptxt 'Lagerdichtung' desc 'Lagerdichtung'</v>
       </c>
@@ -13302,7 +13324,7 @@
       <c r="A75" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="B75" s="23" t="str">
+      <c r="B75" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>BearingType</v>
       </c>
@@ -13320,7 +13342,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G75" s="24" t="str">
+      <c r="G75" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpBearingType</v>
       </c>
@@ -13347,11 +13369,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpBearingType'</v>
       </c>
-      <c r="N75" s="24" t="str">
+      <c r="N75" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'Lagerart'</v>
       </c>
-      <c r="O75" s="24" t="str">
+      <c r="O75" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'Lagerart'</v>
       </c>
@@ -13363,7 +13385,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpBearingType</v>
       </c>
-      <c r="R75" s="24" t="str">
+      <c r="R75" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpBearingTypeUDA Rptxt 'Lagerart' desc 'Lagerart'</v>
       </c>
@@ -13372,7 +13394,7 @@
       <c r="A76" s="22" t="s">
         <v>307</v>
       </c>
-      <c r="B76" s="23" t="str">
+      <c r="B76" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>LubricationTypeDriveSide</v>
       </c>
@@ -13390,7 +13412,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G76" s="24" t="str">
+      <c r="G76" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpLubricationTypeDriveSide</v>
       </c>
@@ -13417,11 +13439,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpLubricationTypeDriveSide'</v>
       </c>
-      <c r="N76" s="24" t="str">
+      <c r="N76" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'Schmierart Antriebsseite'</v>
       </c>
-      <c r="O76" s="24" t="str">
+      <c r="O76" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'Schmierart Antriebsseite'</v>
       </c>
@@ -13433,7 +13455,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpLubricationTypeDriveSide</v>
       </c>
-      <c r="R76" s="24" t="str">
+      <c r="R76" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpLubricationTypeDriveSideUDA Rptxt 'Schmierart Antriebsseite' desc 'Schmierart Antriebsseite'</v>
       </c>
@@ -13442,7 +13464,7 @@
       <c r="A77" s="21" t="s">
         <v>308</v>
       </c>
-      <c r="B77" s="23" t="str">
+      <c r="B77" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>LubricatantControlSystem</v>
       </c>
@@ -13460,7 +13482,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G77" s="24" t="str">
+      <c r="G77" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpLubricatantControlSystem</v>
       </c>
@@ -13487,11 +13509,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpLubricatantControlSystem'</v>
       </c>
-      <c r="N77" s="24" t="str">
+      <c r="N77" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'Schmiermittelüberwachung'</v>
       </c>
-      <c r="O77" s="24" t="str">
+      <c r="O77" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'Schmiermittelüberwachung'</v>
       </c>
@@ -13503,7 +13525,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpLubricatantControlSystem</v>
       </c>
-      <c r="R77" s="24" t="str">
+      <c r="R77" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpLubricatantControlSystemUDA Rptxt 'Schmiermittelüberwachung' desc 'Schmiermittelüberwachung'</v>
       </c>
@@ -13512,7 +13534,7 @@
       <c r="A78" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="B78" s="23" t="str">
+      <c r="B78" s="7" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(EQUI[[#This Row],[Description]]," ",""),"ä","ae"),"(",""),")","")</f>
         <v>CoolingBearingSupport</v>
       </c>
@@ -13530,7 +13552,7 @@
         <f>EQUI[[#Headers],[UDA]]</f>
         <v>UDA</v>
       </c>
-      <c r="G78" s="24" t="str">
+      <c r="G78" s="6" t="str">
         <f>"Tg"&amp;EQUI[[#This Row],[UDET desc]]&amp;EQUI[[#This Row],[Desc E3D]]</f>
         <v>TgPumpCoolingBearingSupport</v>
       </c>
@@ -13557,11 +13579,11 @@
         <f t="shared" si="11"/>
         <v>udname 'TgPumpCoolingBearingSupport'</v>
       </c>
-      <c r="N78" s="24" t="str">
+      <c r="N78" s="6" t="str">
         <f>"Rptxt '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>Rptxt 'Lagerträgerkühlung'</v>
       </c>
-      <c r="O78" s="24" t="str">
+      <c r="O78" s="6" t="str">
         <f>"desc '"&amp;EQUI[[#This Row],[UDA desc]]&amp;"'"</f>
         <v>desc 'Lagerträgerkühlung'</v>
       </c>
@@ -13573,7 +13595,7 @@
         <f t="shared" si="13"/>
         <v>new attcol DbAttribute :TgPumpCoolingBearingSupport</v>
       </c>
-      <c r="R78" s="24" t="str">
+      <c r="R78" s="6" t="str">
         <f t="shared" si="14"/>
         <v>/TgPumpCoolingBearingSupportUDA Rptxt 'Lagerträgerkühlung' desc 'Lagerträgerkühlung'</v>
       </c>

</xml_diff>